<commit_message>
dropped id10184 and id10190, word doc - rectified constraint in dates; included >=id10021 instead of >id10021
</commit_message>
<xml_diff>
--- a/WHOVA2016_v1_5_2_ODK_HB_2019_revision2.xlsx
+++ b/WHOVA2016_v1_5_2_ODK_HB_2019_revision2.xlsx
@@ -18,7 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="_2016survey">survey!$A$1:$O$608</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">survey!$A$1:$O$65</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">survey!$A$1:$A$612</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -12218,8 +12218,8 @@
   <dimension ref="A1:Q612"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A253" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C245" sqref="C245"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15.6" customHeight="1"/>
@@ -26388,7 +26388,6 @@
       <c r="F612" s="17"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:O65"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
added revision 3 which we have removed constraints in 10439-10441 and added .<=today() for 10071
</commit_message>
<xml_diff>
--- a/WHOVA2016_v1_5_2_ODK_HB_2019_revision2.xlsx
+++ b/WHOVA2016_v1_5_2_ODK_HB_2019_revision2.xlsx
@@ -11143,10 +11143,10 @@
     <t>if(${Id10020}='yes' and ${Id10022}='yes',.&gt;=${Id10021} and .&lt;=${Id10023}, .&lt;=${Id10023} or .&lt;=${Id10024})</t>
   </si>
   <si>
-    <t>if(${Id10020}='yes' and ${Id10022}='yes',.&gt;=${Id10021} and .&gt;=${Id10023}, .&gt;=${Id10023} or .&gt;=${Id10024})</t>
-  </si>
-  <si>
     <t xml:space="preserve"> if(${Id10020}='yes' and ${Id10022}='yes',.&gt;=${Id10021} and .&lt;=${Id10023}, .&lt;=${Id10023} or .&lt;=${Id10024})</t>
+  </si>
+  <si>
+    <t>if(${Id10020}='yes' and ${Id10022}='yes',.&gt;=${Id10021} and .&gt;=${Id10023}, (.&gt;=${Id10023} or .&gt;=${Id10024}) and .&lt;=today())</t>
   </si>
 </sst>
 </file>
@@ -12217,9 +12217,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q612"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D37" sqref="D37"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A75" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M98" sqref="M98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15.6" customHeight="1"/>
@@ -13951,7 +13951,7 @@
         <v>3602</v>
       </c>
       <c r="M81" s="66" t="s">
-        <v>3668</v>
+        <v>3667</v>
       </c>
     </row>
     <row r="82" spans="1:13" s="1" customFormat="1" ht="15.6" customHeight="1">
@@ -14280,7 +14280,7 @@
         <v>3602</v>
       </c>
       <c r="M98" t="s">
-        <v>3667</v>
+        <v>3668</v>
       </c>
     </row>
     <row r="99" spans="1:15" s="1" customFormat="1" ht="15.6" customHeight="1">

</xml_diff>